<commit_message>
Removal of json example & update URL
</commit_message>
<xml_diff>
--- a/DanAKS_export_v1_0_0.xlsx
+++ b/DanAKS_export_v1_0_0.xlsx
@@ -488,19 +488,24 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Observation</t>
+          <t>Diagnosis</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>CardiacArrestAfter12h</t>
+          <t>VerifiedDiagnosis</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>True</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="D3" t="inlineStr">
         <is>
-          <t>ResultValue</t>
+          <t>DiagnosisType</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -510,12 +515,17 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Hjertestop senere end 12 timer efter indlæggelse.</t>
+          <t>Den endelige diagnose verificeret af kardiolog ved udskrivelse.</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Enums/Udfald: | "ja" | "nej" | "ikke_relevant" | </t>
+          <t xml:space="preserve">Enums/Udfald: | "di200" | "di213a" | "di213b" | "di213c" | "di214" | "ikke_aks" | </t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>True</t>
         </is>
       </c>
     </row>
@@ -527,7 +537,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>LVEF</t>
+          <t>CardiogenicShockAfter12h</t>
         </is>
       </c>
     </row>
@@ -539,17 +549,17 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Integer</t>
+          <t>str, Enum</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Se webservice dokumentation.</t>
+          <t>Kardiogent shock senere end 12 timer efter indlæggelse.</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Greater than or equal to: 0 | Less than or equal to: 100</t>
+          <t xml:space="preserve">Enums/Udfald: | "ja" | "nej" | "ikke_relevant" | </t>
         </is>
       </c>
     </row>
@@ -561,14 +571,14 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>CardiacEcho</t>
+          <t>CardiacArrestWithin12h</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="D7" t="inlineStr">
         <is>
-          <t>StatusCode</t>
+          <t>ResultValue</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -578,7 +588,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Er Ekkokardiografi udført?</t>
+          <t>Se webservice dokumentation.</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -595,7 +605,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>CardiogenicShockAfter12h</t>
+          <t>AcuteHeartFailureKillipClass</t>
         </is>
       </c>
     </row>
@@ -612,12 +622,12 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Kardiogent shock senere end 12 timer efter indlæggelse.</t>
+          <t>Killip klasse indenfor 12 timer efter indlæggelse.</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Enums/Udfald: | "ja" | "nej" | "ikke_relevant" | </t>
+          <t xml:space="preserve">Enums/Udfald: | "killip_klasse1" | "killip_klasse2" | "killip_klasse3" | "killip_klasse4" | </t>
         </is>
       </c>
     </row>
@@ -629,7 +639,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>AcuteHeartFailureKillipClass</t>
+          <t>LVEF</t>
         </is>
       </c>
     </row>
@@ -641,17 +651,17 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>str, Enum</t>
+          <t>Integer</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Killip klasse indenfor 12 timer efter indlæggelse.</t>
+          <t>Se webservice dokumentation.</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t xml:space="preserve">Enums/Udfald: | "killip_klasse1" | "killip_klasse2" | "killip_klasse3" | "killip_klasse4" | </t>
+          <t>Greater than or equal to: 0 | Less than or equal to: 100</t>
         </is>
       </c>
     </row>
@@ -663,7 +673,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>CardiacArrestWithin12h</t>
+          <t>CardiacArrestAfter12h</t>
         </is>
       </c>
     </row>
@@ -680,36 +690,31 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Se webservice dokumentation.</t>
+          <t>Hjertestop senere end 12 timer efter indlæggelse.</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t xml:space="preserve">Enums/Udfald: | "ja" | "nej" | </t>
+          <t xml:space="preserve">Enums/Udfald: | "ja" | "nej" | "ikke_relevant" | </t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Diagnosis</t>
+          <t>Observation</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>VerifiedDiagnosis</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>True</t>
+          <t>CardiacEcho</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="D15" t="inlineStr">
         <is>
-          <t>DiagnosisType</t>
+          <t>StatusCode</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -719,17 +724,12 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Den endelige diagnose verificeret af kardiolog ved udskrivelse.</t>
+          <t>Er Ekkokardiografi udført?</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t xml:space="preserve">Enums/Udfald: | "di200" | "di213a" | "di213b" | "di213c" | "di214" | "ikke_aks" | </t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>True</t>
+          <t xml:space="preserve">Enums/Udfald: | "ja" | "nej" | </t>
         </is>
       </c>
     </row>

</xml_diff>